<commit_message>
Extended Config to 2K, refactors Tasks and Config
</commit_message>
<xml_diff>
--- a/final-project/Docs/Face Angles.xlsx
+++ b/final-project/Docs/Face Angles.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://athousandprojects-my.sharepoint.com/personal/graeme_athousandprojects_com/Documents/Study/Making Embedded Systems/making-embedded-projects/final-project/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="8_{001D23B9-69B6-4F06-BAEA-CFA795CAD8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{423C316A-9F7B-421F-84EC-8C6FCEA598A2}"/>
+  <xr:revisionPtr revIDLastSave="176" documentId="8_{001D23B9-69B6-4F06-BAEA-CFA795CAD8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59F7A2E8-B499-4AFB-8FF1-883112ABB1F1}"/>
   <bookViews>
-    <workbookView xWindow="29985" yWindow="1020" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{615AABFA-D9F8-4798-8FA6-969E46F85DBB}"/>
+    <workbookView xWindow="31455" yWindow="1815" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{615AABFA-D9F8-4798-8FA6-969E46F85DBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Angles" sheetId="1" r:id="rId1"/>
     <sheet name="Config" sheetId="2" r:id="rId2"/>
     <sheet name="System State machine" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="50">
   <si>
     <t>Face</t>
   </si>
@@ -139,6 +140,54 @@
   </si>
   <si>
     <t>TIMER INT</t>
+  </si>
+  <si>
+    <t>Initialisation</t>
+  </si>
+  <si>
+    <t>Set Date/Time</t>
+  </si>
+  <si>
+    <t>Enter Task  Config</t>
+  </si>
+  <si>
+    <t>Enter Face Config</t>
+  </si>
+  <si>
+    <t>MOVE_STATE</t>
+  </si>
+  <si>
+    <t>IDLE_STATE</t>
+  </si>
+  <si>
+    <t>NEW_FACE_DETECTED</t>
+  </si>
+  <si>
+    <t>SLEEP_STATE</t>
+  </si>
+  <si>
+    <t>CHANGE_TASK</t>
+  </si>
+  <si>
+    <t>END_TASK</t>
+  </si>
+  <si>
+    <t>static uint16_t SYS_CONFIG_SIZE ;</t>
+  </si>
+  <si>
+    <t>static uint16_t SYS_CONFIG_ALL_SIZE;</t>
+  </si>
+  <si>
+    <t>static uint16_t SYS_CONFIG_SIZE_TASK;</t>
+  </si>
+  <si>
+    <t>static uint16_t SYS_CONFIG_SIZE_DODEC;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Where is </t>
+  </si>
+  <si>
+    <t>plud Checksum</t>
   </si>
 </sst>
 </file>
@@ -1411,7 +1460,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D6" si="0">C2*8</f>
+        <f t="shared" ref="D2:D5" si="0">C2*8</f>
         <v>8</v>
       </c>
       <c r="E2">
@@ -1556,15 +1605,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1F8812-A739-45D4-ABFD-B6C85B2259E7}">
-  <dimension ref="C1:E1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>31</v>
       </c>
@@ -1573,6 +1625,251 @@
       </c>
       <c r="E1" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8BF0F1-1847-40BE-B07E-F183D7EF20B2}">
+  <dimension ref="A2:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2">
+        <v>896</v>
+      </c>
+      <c r="C2">
+        <f>B2/4</f>
+        <v>224</v>
+      </c>
+      <c r="D2">
+        <f>B2*8</f>
+        <v>7168</v>
+      </c>
+      <c r="E2">
+        <f>D2/32</f>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>904</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C5" si="0">B3/4</f>
+        <v>226</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D5" si="1">B3*8</f>
+        <v>7232</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E5" si="2">D3/32</f>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4">
+        <v>800</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>6400</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5">
+        <v>96</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>768</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8">
+        <f>B3-B2</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10">
+        <v>896</v>
+      </c>
+      <c r="C10">
+        <f>B10/4</f>
+        <v>224</v>
+      </c>
+      <c r="D10">
+        <f>B10*8</f>
+        <v>7168</v>
+      </c>
+      <c r="E10">
+        <f>D10/32</f>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11">
+        <v>900</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:C13" si="3">B11/4</f>
+        <v>225</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:D13" si="4">B11*8</f>
+        <v>7200</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ref="E11:E13" si="5">D11/32</f>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12">
+        <v>800</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="4"/>
+        <v>6400</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="5"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13">
+        <v>96</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="4"/>
+        <v>768</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Busy with State Table Controller
</commit_message>
<xml_diff>
--- a/final-project/Docs/Face Angles.xlsx
+++ b/final-project/Docs/Face Angles.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://athousandprojects-my.sharepoint.com/personal/graeme_athousandprojects_com/Documents/Study/Making Embedded Systems/making-embedded-projects/final-project/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="8_{001D23B9-69B6-4F06-BAEA-CFA795CAD8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59F7A2E8-B499-4AFB-8FF1-883112ABB1F1}"/>
+  <xr:revisionPtr revIDLastSave="283" documentId="8_{001D23B9-69B6-4F06-BAEA-CFA795CAD8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A00104A6-5FD9-4BA2-A561-009F87CAC83C}"/>
   <bookViews>
-    <workbookView xWindow="31455" yWindow="1815" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{615AABFA-D9F8-4798-8FA6-969E46F85DBB}"/>
+    <workbookView xWindow="3315" yWindow="1515" windowWidth="24240" windowHeight="13575" activeTab="2" xr2:uid="{615AABFA-D9F8-4798-8FA6-969E46F85DBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Angles" sheetId="1" r:id="rId1"/>
     <sheet name="Config" sheetId="2" r:id="rId2"/>
     <sheet name="System State machine" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="51">
   <si>
     <t>Face</t>
   </si>
@@ -133,9 +132,6 @@
     <t>Bytes</t>
   </si>
   <si>
-    <t>Acc INT</t>
-  </si>
-  <si>
     <t>LIPO INT</t>
   </si>
   <si>
@@ -145,49 +141,56 @@
     <t>Initialisation</t>
   </si>
   <si>
-    <t>Set Date/Time</t>
-  </si>
-  <si>
-    <t>Enter Task  Config</t>
-  </si>
-  <si>
-    <t>Enter Face Config</t>
-  </si>
-  <si>
-    <t>MOVE_STATE</t>
-  </si>
-  <si>
-    <t>IDLE_STATE</t>
-  </si>
-  <si>
-    <t>NEW_FACE_DETECTED</t>
-  </si>
-  <si>
-    <t>SLEEP_STATE</t>
-  </si>
-  <si>
-    <t>CHANGE_TASK</t>
-  </si>
-  <si>
-    <t>END_TASK</t>
-  </si>
-  <si>
-    <t>static uint16_t SYS_CONFIG_SIZE ;</t>
-  </si>
-  <si>
-    <t>static uint16_t SYS_CONFIG_ALL_SIZE;</t>
-  </si>
-  <si>
-    <t>static uint16_t SYS_CONFIG_SIZE_TASK;</t>
-  </si>
-  <si>
-    <t>static uint16_t SYS_CONFIG_SIZE_DODEC;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Where is </t>
-  </si>
-  <si>
-    <t>plud Checksum</t>
+    <t>STATE_CONFIG</t>
+  </si>
+  <si>
+    <t>STATE_IDLE</t>
+  </si>
+  <si>
+    <t>STATE_CHANGE_TASK</t>
+  </si>
+  <si>
+    <t>STATE_END_TASK</t>
+  </si>
+  <si>
+    <t>STATE_BATTERY_TEST</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>User in config mode, 
+Automaticn face detection disabled</t>
+  </si>
+  <si>
+    <t>Set up new Task relating to new face</t>
+  </si>
+  <si>
+    <t>Dodeca has been placed on STOP Face</t>
+  </si>
+  <si>
+    <t>Test and Display Battery</t>
+  </si>
+  <si>
+    <t>STATE_SLEEP</t>
+  </si>
+  <si>
+    <t>Dodeca is Sleeping</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>NEW FACE</t>
+  </si>
+  <si>
+    <t>STATE_UPDATE_TASK</t>
+  </si>
+  <si>
+    <t>Nothing happening until it does</t>
+  </si>
+  <si>
+    <t>DONE/TimeOut</t>
   </si>
 </sst>
 </file>
@@ -211,7 +214,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,6 +245,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -264,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -273,6 +288,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1426,7 +1451,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,274 +1630,177 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1F8812-A739-45D4-ABFD-B6C85B2259E7}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="1" max="1" width="26" style="8" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B8" s="9" t="s">
         <v>43</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8BF0F1-1847-40BE-B07E-F183D7EF20B2}">
-  <dimension ref="A2:E15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2">
-        <v>896</v>
-      </c>
-      <c r="C2">
-        <f>B2/4</f>
-        <v>224</v>
-      </c>
-      <c r="D2">
-        <f>B2*8</f>
-        <v>7168</v>
-      </c>
-      <c r="E2">
-        <f>D2/32</f>
-        <v>224</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3">
-        <v>904</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C5" si="0">B3/4</f>
-        <v>226</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D5" si="1">B3*8</f>
-        <v>7232</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E5" si="2">D3/32</f>
-        <v>226</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4">
-        <v>800</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="1"/>
-        <v>6400</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5">
-        <v>96</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="1"/>
-        <v>768</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8">
-        <f>B3-B2</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10">
-        <v>896</v>
-      </c>
-      <c r="C10">
-        <f>B10/4</f>
-        <v>224</v>
-      </c>
-      <c r="D10">
-        <f>B10*8</f>
-        <v>7168</v>
-      </c>
-      <c r="E10">
-        <f>D10/32</f>
-        <v>224</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11">
-        <v>900</v>
-      </c>
-      <c r="C11">
-        <f t="shared" ref="C11:C13" si="3">B11/4</f>
-        <v>225</v>
-      </c>
-      <c r="D11">
-        <f t="shared" ref="D11:D13" si="4">B11*8</f>
-        <v>7200</v>
-      </c>
-      <c r="E11">
-        <f t="shared" ref="E11:E13" si="5">D11/32</f>
-        <v>225</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12">
-        <v>800</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="3"/>
-        <v>200</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="4"/>
-        <v>6400</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="5"/>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13">
-        <v>96</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="3"/>
-        <v>24</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="4"/>
-        <v>768</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="5"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>